<commit_message>
Capm y modelo mercado
</commit_message>
<xml_diff>
--- a/Calendario Curso.xlsx
+++ b/Calendario Curso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dauam-my.sharepoint.com/personal/alfonso_santos_uam_es/Documents/Cursos Python/microcredencial-carteras-python-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{ECA2F6F7-C578-4B61-8963-8AC680C6829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF39927-E995-4543-9D1C-F4782DD2F0B3}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{ECA2F6F7-C578-4B61-8963-8AC680C6829E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E16DF586-1382-4FFB-893E-F90B1A338BE3}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Level I - Nuevo" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>LUNES</t>
   </si>
@@ -101,10 +100,6 @@
     <t>APT</t>
   </si>
   <si>
-    <t>Revisión Práctica
-APT</t>
-  </si>
-  <si>
     <t>Repaso CVXpy3.4 Markowitz
 Tobin</t>
   </si>
@@ -117,18 +112,15 @@
 CAPM</t>
   </si>
   <si>
-    <t>Modelo Mercado</t>
-  </si>
-  <si>
-    <t>APT
-Explicación Práctica</t>
-  </si>
-  <si>
     <t xml:space="preserve">VAR
 </t>
   </si>
   <si>
     <t>PROBLEMAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo Mercado
+</t>
   </si>
 </sst>
 </file>
@@ -562,7 +554,7 @@
   <dimension ref="A1:J1026"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="200" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -754,11 +746,11 @@
     </row>
     <row r="9" spans="1:10" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>9</v>
@@ -870,12 +862,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="12" t="s">
-        <v>24</v>
+      <c r="C15" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>25</v>
@@ -931,7 +921,7 @@
     </row>
     <row r="18" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="12" t="s">
@@ -989,11 +979,11 @@
     </row>
     <row r="21" spans="1:9" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>9</v>

</xml_diff>